<commit_message>
FType 4 minimum -637
</commit_message>
<xml_diff>
--- a/PSO_Auswertung.xlsx
+++ b/PSO_Auswertung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="89">
   <si>
     <t>Testfunktion</t>
   </si>
@@ -202,6 +202,90 @@
   </si>
   <si>
     <t>-0.001 bis 0.001</t>
+  </si>
+  <si>
+    <t>4 von 10.000</t>
+  </si>
+  <si>
+    <t>14 von 100.000</t>
+  </si>
+  <si>
+    <t>1 von 100.000</t>
+  </si>
+  <si>
+    <t>46 von 100.000</t>
+  </si>
+  <si>
+    <t>72 von 100.000</t>
+  </si>
+  <si>
+    <t>63 von 100.000</t>
+  </si>
+  <si>
+    <t>9 von 100.000</t>
+  </si>
+  <si>
+    <t>-5  bis 5</t>
+  </si>
+  <si>
+    <t>44 von 100.000</t>
+  </si>
+  <si>
+    <t>65 von 100.000</t>
+  </si>
+  <si>
+    <t>187 von 100.000</t>
+  </si>
+  <si>
+    <t>160 von 100.000</t>
+  </si>
+  <si>
+    <t>0.000001</t>
+  </si>
+  <si>
+    <t>66 von 100.000</t>
+  </si>
+  <si>
+    <t>74 von 100.000</t>
+  </si>
+  <si>
+    <t>83 von 100.000</t>
+  </si>
+  <si>
+    <t>85 von 100.000</t>
+  </si>
+  <si>
+    <t>55 von 100.000</t>
+  </si>
+  <si>
+    <t>47 von 100.000</t>
+  </si>
+  <si>
+    <t>20 von 100.000</t>
+  </si>
+  <si>
+    <t>49 von 100.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.001 bis 0.001 </t>
+  </si>
+  <si>
+    <t>245 von 100.000</t>
+  </si>
+  <si>
+    <t>45 von 100.000</t>
+  </si>
+  <si>
+    <t>105 von 100.000</t>
+  </si>
+  <si>
+    <t>87 von 100.000</t>
+  </si>
+  <si>
+    <t>92 von 100.000</t>
+  </si>
+  <si>
+    <t>23 von 100.000</t>
   </si>
 </sst>
 </file>
@@ -217,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,25 +316,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -275,14 +341,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -597,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L74"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,38 +1772,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>3</v>
-      </c>
-      <c r="C33" s="3" t="s">
+    <row r="33" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>3</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="6">
         <v>66</v>
       </c>
-      <c r="E33" s="3">
-        <v>500</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="E33" s="6">
+        <v>500</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="H33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="6">
         <v>0.75</v>
       </c>
-      <c r="J33" s="3">
-        <v>1</v>
-      </c>
-      <c r="K33" s="3">
+      <c r="J33" s="6">
+        <v>1</v>
+      </c>
+      <c r="K33" s="6">
         <v>0.5</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1885,38 +1947,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="3">
-        <v>3</v>
-      </c>
-      <c r="C38" s="3" t="s">
+    <row r="38" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>3</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="6">
         <v>63</v>
       </c>
-      <c r="E38" s="3">
-        <v>500</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="5" t="s">
+      <c r="E38" s="6">
+        <v>500</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="3">
+      <c r="H38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="6">
         <v>0.75</v>
       </c>
-      <c r="J38" s="3">
-        <v>1</v>
-      </c>
-      <c r="K38" s="3">
+      <c r="J38" s="6">
+        <v>1</v>
+      </c>
+      <c r="K38" s="6">
         <v>0.5</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2305,73 +2367,73 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="3">
-        <v>3</v>
-      </c>
-      <c r="C50" s="3" t="s">
+    <row r="50" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="6">
+        <v>3</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="6">
         <v>64</v>
       </c>
-      <c r="E50" s="3">
-        <v>500</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="5" t="s">
+      <c r="E50" s="6">
+        <v>500</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" s="3">
+      <c r="H50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="6">
         <v>0.7</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="6">
         <v>0.5</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="6">
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="3">
-        <v>3</v>
-      </c>
-      <c r="C51" s="3" t="s">
+    <row r="51" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="6">
+        <v>3</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="6">
         <v>66</v>
       </c>
-      <c r="E51" s="3">
-        <v>500</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="5" t="s">
+      <c r="E51" s="6">
+        <v>500</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="3">
+      <c r="H51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="6">
         <v>0.7</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="6">
         <v>0.5</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -2480,38 +2542,38 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="9">
-        <v>3</v>
-      </c>
-      <c r="C55" s="9" t="s">
+    <row r="55" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="6">
+        <v>3</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="6">
         <v>53</v>
       </c>
-      <c r="E55" s="9">
-        <v>500</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="10" t="s">
+      <c r="E55" s="6">
+        <v>500</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H55" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I55" s="9">
+      <c r="H55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55" s="6">
         <v>0.7</v>
       </c>
-      <c r="J55" s="9">
+      <c r="J55" s="6">
         <v>1.01</v>
       </c>
-      <c r="K55" s="9">
+      <c r="K55" s="6">
         <v>0.5</v>
       </c>
-      <c r="L55" s="9">
+      <c r="L55" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -2550,17 +2612,17 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="7">
-        <v>3</v>
-      </c>
-      <c r="C57" s="7" t="s">
+    <row r="57" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="6">
+        <v>3</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="6">
         <v>6</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="6">
         <v>500</v>
       </c>
       <c r="F57" s="8" t="s">
@@ -2569,19 +2631,19 @@
       <c r="G57" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H57" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I57" s="7">
+      <c r="H57" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I57" s="6">
         <v>0.7</v>
       </c>
-      <c r="J57" s="7">
+      <c r="J57" s="6">
         <v>1.01</v>
       </c>
-      <c r="K57" s="7">
+      <c r="K57" s="6">
         <v>0.5</v>
       </c>
-      <c r="L57" s="7">
+      <c r="L57" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -2725,38 +2787,38 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="11">
-        <v>3</v>
-      </c>
-      <c r="C62" s="11" t="s">
+    <row r="62" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="6">
+        <v>3</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="6">
         <v>5.5460000000000003</v>
       </c>
-      <c r="E62" s="11">
-        <v>500</v>
-      </c>
-      <c r="F62" s="12" t="s">
+      <c r="E62" s="6">
+        <v>500</v>
+      </c>
+      <c r="F62" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G62" s="12" t="s">
+      <c r="G62" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H62" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I62" s="11">
+      <c r="H62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I62" s="6">
         <v>0.70499999999999996</v>
       </c>
-      <c r="J62" s="11">
+      <c r="J62" s="6">
         <v>1.0109999999999999</v>
       </c>
-      <c r="K62" s="11">
+      <c r="K62" s="6">
         <v>0.505</v>
       </c>
-      <c r="L62" s="11">
+      <c r="L62" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -2900,38 +2962,38 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="67" spans="2:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="13">
-        <v>3</v>
-      </c>
-      <c r="C67" s="13" t="s">
+    <row r="67" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="6">
+        <v>3</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D67" s="13">
+      <c r="D67" s="6">
         <v>4.4870570000000001</v>
       </c>
-      <c r="E67" s="13">
-        <v>500</v>
-      </c>
-      <c r="F67" s="14" t="s">
+      <c r="E67" s="6">
+        <v>500</v>
+      </c>
+      <c r="F67" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H67" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I67" s="13">
+      <c r="H67" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I67" s="6">
         <v>0.70499999999999996</v>
       </c>
-      <c r="J67" s="13">
+      <c r="J67" s="6">
         <v>1.0109999999999999</v>
       </c>
-      <c r="K67" s="13">
+      <c r="K67" s="6">
         <v>0.505</v>
       </c>
-      <c r="L67" s="13">
+      <c r="L67" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -3145,39 +3207,1824 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="9">
-        <v>3</v>
-      </c>
-      <c r="C74" s="9" t="s">
+    <row r="74" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="6">
+        <v>3</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="6">
         <v>4.1900000000000004</v>
       </c>
-      <c r="E74" s="9">
-        <v>500</v>
-      </c>
-      <c r="F74" s="10" t="s">
+      <c r="E74" s="6">
+        <v>500</v>
+      </c>
+      <c r="F74" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G74" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H74" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74" s="9">
+      <c r="G74" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I74" s="6">
         <v>0.70050000000000001</v>
       </c>
-      <c r="J74" s="9">
+      <c r="J74" s="6">
         <v>1.0101</v>
       </c>
-      <c r="K74" s="9">
+      <c r="K74" s="6">
         <v>0.50049999999999994</v>
       </c>
-      <c r="L74" s="9">
+      <c r="L74" s="6">
         <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75">
+        <v>72</v>
+      </c>
+      <c r="E75">
+        <v>500</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I75">
+        <v>0.70050000000000001</v>
+      </c>
+      <c r="J75">
+        <v>1.0101</v>
+      </c>
+      <c r="K75">
+        <v>0.50049999999999994</v>
+      </c>
+      <c r="L75">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76">
+        <v>3.0114299999999998</v>
+      </c>
+      <c r="E76">
+        <v>500</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I76">
+        <v>0.70004999999999995</v>
+      </c>
+      <c r="J76">
+        <v>1.0100100000000001</v>
+      </c>
+      <c r="K76">
+        <v>0.50004999999999999</v>
+      </c>
+      <c r="L76">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77">
+        <v>5.16</v>
+      </c>
+      <c r="E77">
+        <v>500</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I77">
+        <v>0.70004999999999995</v>
+      </c>
+      <c r="J77">
+        <v>1.0100100000000001</v>
+      </c>
+      <c r="K77">
+        <v>0.50004999999999999</v>
+      </c>
+      <c r="L77">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79">
+        <v>54.569000000000003</v>
+      </c>
+      <c r="E79">
+        <v>500</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H79" t="s">
+        <v>12</v>
+      </c>
+      <c r="I79">
+        <v>0.7</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>0.5</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80">
+        <v>87</v>
+      </c>
+      <c r="E80">
+        <v>500</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H80" t="s">
+        <v>12</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81">
+        <v>110</v>
+      </c>
+      <c r="E81">
+        <v>500</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H81" t="s">
+        <v>12</v>
+      </c>
+      <c r="I81">
+        <v>2</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82">
+        <v>102</v>
+      </c>
+      <c r="E82">
+        <v>500</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H82" t="s">
+        <v>12</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>2</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>4</v>
+      </c>
+      <c r="C83" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83">
+        <v>88</v>
+      </c>
+      <c r="E83">
+        <v>500</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H83" t="s">
+        <v>12</v>
+      </c>
+      <c r="I83">
+        <v>0.5</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>4</v>
+      </c>
+      <c r="C84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84">
+        <v>28.7194</v>
+      </c>
+      <c r="E84">
+        <v>500</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H84" t="s">
+        <v>12</v>
+      </c>
+      <c r="I84">
+        <v>0.5</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <v>0.5</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D85">
+        <v>179</v>
+      </c>
+      <c r="E85">
+        <v>500</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H85" t="s">
+        <v>12</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86">
+        <v>87</v>
+      </c>
+      <c r="E86">
+        <v>500</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H86" t="s">
+        <v>12</v>
+      </c>
+      <c r="I86">
+        <v>0.5</v>
+      </c>
+      <c r="J86">
+        <v>0.5</v>
+      </c>
+      <c r="K86">
+        <v>0.5</v>
+      </c>
+      <c r="L86">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87">
+        <v>89</v>
+      </c>
+      <c r="E87">
+        <v>500</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H87" t="s">
+        <v>12</v>
+      </c>
+      <c r="I87">
+        <v>0.5</v>
+      </c>
+      <c r="J87">
+        <v>0.5</v>
+      </c>
+      <c r="K87">
+        <v>0.5</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>4</v>
+      </c>
+      <c r="C88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D88">
+        <v>78</v>
+      </c>
+      <c r="E88">
+        <v>500</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H88" t="s">
+        <v>12</v>
+      </c>
+      <c r="I88">
+        <v>0.5</v>
+      </c>
+      <c r="J88">
+        <v>0.8</v>
+      </c>
+      <c r="K88">
+        <v>0.8</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>27</v>
+      </c>
+      <c r="D89">
+        <v>199</v>
+      </c>
+      <c r="E89">
+        <v>500</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H89" t="s">
+        <v>12</v>
+      </c>
+      <c r="I89" s="1">
+        <f>I96-0.5</f>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="J89" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="K89" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>64</v>
+      </c>
+      <c r="D90">
+        <v>-595.11369999999999</v>
+      </c>
+      <c r="E90">
+        <v>500</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H90" t="s">
+        <v>12</v>
+      </c>
+      <c r="I90">
+        <v>0.5</v>
+      </c>
+      <c r="J90">
+        <v>0.8</v>
+      </c>
+      <c r="K90">
+        <v>0.8</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s">
+        <v>65</v>
+      </c>
+      <c r="D91">
+        <v>-609.27750000000003</v>
+      </c>
+      <c r="E91">
+        <v>500</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H91" t="s">
+        <v>12</v>
+      </c>
+      <c r="I91">
+        <v>0.5</v>
+      </c>
+      <c r="J91">
+        <v>0.8</v>
+      </c>
+      <c r="K91">
+        <v>0.8</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>66</v>
+      </c>
+      <c r="D92" s="1">
+        <v>-609.27674999999999</v>
+      </c>
+      <c r="E92">
+        <v>500</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H92" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92">
+        <v>0.5</v>
+      </c>
+      <c r="J92">
+        <v>0.8</v>
+      </c>
+      <c r="K92">
+        <v>0.8</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93">
+        <v>-456.14429999999999</v>
+      </c>
+      <c r="E93">
+        <v>500</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H93" t="s">
+        <v>12</v>
+      </c>
+      <c r="I93">
+        <v>0.505</v>
+      </c>
+      <c r="J93">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="K93">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="L93">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94" t="s">
+        <v>67</v>
+      </c>
+      <c r="D94">
+        <v>-551.64239999999995</v>
+      </c>
+      <c r="E94">
+        <v>500</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H94" t="s">
+        <v>12</v>
+      </c>
+      <c r="I94">
+        <v>0.505</v>
+      </c>
+      <c r="J94">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="K94">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="L94">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>4</v>
+      </c>
+      <c r="C95" t="s">
+        <v>69</v>
+      </c>
+      <c r="D95">
+        <v>-595.11387000000002</v>
+      </c>
+      <c r="E95">
+        <v>500</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H95" t="s">
+        <v>12</v>
+      </c>
+      <c r="I95">
+        <v>0.505</v>
+      </c>
+      <c r="J95">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="K95">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="L95">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="3">
+        <v>4</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D96" s="3">
+        <v>-623.41399999999999</v>
+      </c>
+      <c r="E96" s="3">
+        <v>500</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I96" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="J96" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="K96" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="L96" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97" t="s">
+        <v>71</v>
+      </c>
+      <c r="D97">
+        <v>-566.86699999999996</v>
+      </c>
+      <c r="E97">
+        <v>500</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H97" t="s">
+        <v>12</v>
+      </c>
+      <c r="I97">
+        <v>0.49</v>
+      </c>
+      <c r="J97">
+        <v>0.79</v>
+      </c>
+      <c r="K97">
+        <v>0.8</v>
+      </c>
+      <c r="L97">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>4</v>
+      </c>
+      <c r="C98" t="s">
+        <v>72</v>
+      </c>
+      <c r="D98">
+        <v>-595.14121999999998</v>
+      </c>
+      <c r="E98">
+        <v>500</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H98" t="s">
+        <v>12</v>
+      </c>
+      <c r="I98">
+        <v>0.49</v>
+      </c>
+      <c r="J98">
+        <v>0.79</v>
+      </c>
+      <c r="K98">
+        <v>0.8</v>
+      </c>
+      <c r="L98">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99" t="s">
+        <v>74</v>
+      </c>
+      <c r="D99">
+        <v>-609.27660000000003</v>
+      </c>
+      <c r="E99">
+        <v>500</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H99" t="s">
+        <v>73</v>
+      </c>
+      <c r="I99">
+        <v>0.49</v>
+      </c>
+      <c r="J99">
+        <v>0.79</v>
+      </c>
+      <c r="K99">
+        <v>0.8</v>
+      </c>
+      <c r="L99">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100">
+        <v>-425.28570000000002</v>
+      </c>
+      <c r="E100">
+        <v>500</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H100" t="s">
+        <v>73</v>
+      </c>
+      <c r="I100">
+        <v>0.48</v>
+      </c>
+      <c r="J100">
+        <v>0.78</v>
+      </c>
+      <c r="K100">
+        <v>0.78</v>
+      </c>
+      <c r="L100">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101" t="s">
+        <v>20</v>
+      </c>
+      <c r="D101" s="1">
+        <v>-438.62799999999999</v>
+      </c>
+      <c r="E101">
+        <v>500</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H101" t="s">
+        <v>73</v>
+      </c>
+      <c r="I101">
+        <v>0.48</v>
+      </c>
+      <c r="J101">
+        <v>0.78</v>
+      </c>
+      <c r="K101">
+        <v>0.78</v>
+      </c>
+      <c r="L101">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102" t="s">
+        <v>36</v>
+      </c>
+      <c r="D102">
+        <v>-564.995</v>
+      </c>
+      <c r="E102">
+        <v>500</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H102" t="s">
+        <v>73</v>
+      </c>
+      <c r="I102">
+        <v>0.48</v>
+      </c>
+      <c r="J102">
+        <v>0.78</v>
+      </c>
+      <c r="K102">
+        <v>0.78</v>
+      </c>
+      <c r="L102">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>4</v>
+      </c>
+      <c r="C103" t="s">
+        <v>75</v>
+      </c>
+      <c r="D103">
+        <v>-566.86109999999996</v>
+      </c>
+      <c r="E103">
+        <v>500</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H103" t="s">
+        <v>73</v>
+      </c>
+      <c r="I103">
+        <v>0.48</v>
+      </c>
+      <c r="J103">
+        <v>0.78</v>
+      </c>
+      <c r="K103">
+        <v>0.78</v>
+      </c>
+      <c r="L103">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104" t="s">
+        <v>76</v>
+      </c>
+      <c r="D104">
+        <v>-580.93709999999999</v>
+      </c>
+      <c r="E104">
+        <v>500</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H104" t="s">
+        <v>73</v>
+      </c>
+      <c r="I104">
+        <v>0.48</v>
+      </c>
+      <c r="J104">
+        <v>0.78</v>
+      </c>
+      <c r="K104">
+        <v>0.78</v>
+      </c>
+      <c r="L104">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>77</v>
+      </c>
+      <c r="D105">
+        <v>-609.27790000000005</v>
+      </c>
+      <c r="E105">
+        <v>500</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H105" t="s">
+        <v>73</v>
+      </c>
+      <c r="I105">
+        <v>0.48</v>
+      </c>
+      <c r="J105">
+        <v>0.78</v>
+      </c>
+      <c r="K105">
+        <v>0.78</v>
+      </c>
+      <c r="L105">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106">
+        <v>-464.38299999999998</v>
+      </c>
+      <c r="E106">
+        <v>500</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H106" t="s">
+        <v>73</v>
+      </c>
+      <c r="I106">
+        <v>0.48</v>
+      </c>
+      <c r="J106">
+        <v>0.78</v>
+      </c>
+      <c r="K106">
+        <v>0.79</v>
+      </c>
+      <c r="L106">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>4</v>
+      </c>
+      <c r="C107" t="s">
+        <v>78</v>
+      </c>
+      <c r="D107">
+        <v>-566.86469999999997</v>
+      </c>
+      <c r="E107">
+        <v>500</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H107" t="s">
+        <v>73</v>
+      </c>
+      <c r="I107">
+        <v>0.48</v>
+      </c>
+      <c r="J107">
+        <v>0.78</v>
+      </c>
+      <c r="K107">
+        <v>0.79</v>
+      </c>
+      <c r="L107">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="3">
+        <v>4</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D108" s="3">
+        <v>-623.37649999999996</v>
+      </c>
+      <c r="E108" s="3">
+        <v>500</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I108" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="J108" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="K108" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="L108" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>80</v>
+      </c>
+      <c r="D109">
+        <v>-610.32100000000003</v>
+      </c>
+      <c r="E109">
+        <v>500</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H109" t="s">
+        <v>73</v>
+      </c>
+      <c r="I109">
+        <v>0.48</v>
+      </c>
+      <c r="J109">
+        <v>0.77</v>
+      </c>
+      <c r="K109">
+        <v>0.79</v>
+      </c>
+      <c r="L109">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="9">
+        <v>4</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D110" s="9">
+        <v>-637.54690000000005</v>
+      </c>
+      <c r="E110" s="9">
+        <v>500</v>
+      </c>
+      <c r="F110" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H110" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I110" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="J110" s="9">
+        <v>0.77</v>
+      </c>
+      <c r="K110" s="9">
+        <v>0.79</v>
+      </c>
+      <c r="L110" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>4</v>
+      </c>
+      <c r="C111" t="s">
+        <v>70</v>
+      </c>
+      <c r="D111">
+        <v>-581.00239999999997</v>
+      </c>
+      <c r="E111">
+        <v>500</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H111" t="s">
+        <v>73</v>
+      </c>
+      <c r="I111">
+        <v>0.48</v>
+      </c>
+      <c r="J111">
+        <v>0.76</v>
+      </c>
+      <c r="K111">
+        <v>0.79</v>
+      </c>
+      <c r="L111">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>4</v>
+      </c>
+      <c r="C112" t="s">
+        <v>83</v>
+      </c>
+      <c r="D112">
+        <v>-609.26499999999999</v>
+      </c>
+      <c r="E112">
+        <v>500</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H112" t="s">
+        <v>73</v>
+      </c>
+      <c r="I112">
+        <v>0.48</v>
+      </c>
+      <c r="J112">
+        <v>0.76</v>
+      </c>
+      <c r="K112">
+        <v>0.79</v>
+      </c>
+      <c r="L112">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>4</v>
+      </c>
+      <c r="C113" t="s">
+        <v>75</v>
+      </c>
+      <c r="D113">
+        <v>-566.86776999999995</v>
+      </c>
+      <c r="E113">
+        <v>500</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H113" t="s">
+        <v>73</v>
+      </c>
+      <c r="I113">
+        <v>0.48</v>
+      </c>
+      <c r="J113">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="K113">
+        <v>0.79</v>
+      </c>
+      <c r="L113">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>4</v>
+      </c>
+      <c r="C114" t="s">
+        <v>84</v>
+      </c>
+      <c r="D114">
+        <v>-580.96581000000003</v>
+      </c>
+      <c r="E114">
+        <v>500</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H114" t="s">
+        <v>73</v>
+      </c>
+      <c r="I114">
+        <v>0.48</v>
+      </c>
+      <c r="J114">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="K114">
+        <v>0.79</v>
+      </c>
+      <c r="L114">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>4</v>
+      </c>
+      <c r="C115" t="s">
+        <v>85</v>
+      </c>
+      <c r="D115">
+        <v>-609.27790000000005</v>
+      </c>
+      <c r="E115">
+        <v>500</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H115" t="s">
+        <v>73</v>
+      </c>
+      <c r="I115">
+        <v>0.48</v>
+      </c>
+      <c r="J115">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="K115">
+        <v>0.79</v>
+      </c>
+      <c r="L115">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="3">
+        <v>4</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D116" s="3">
+        <v>-623.41463999999996</v>
+      </c>
+      <c r="E116" s="3">
+        <v>500</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I116" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="J116" s="3">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="K116" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="L116" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117" t="s">
+        <v>31</v>
+      </c>
+      <c r="D117">
+        <v>-540.57500000000005</v>
+      </c>
+      <c r="E117">
+        <v>500</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H117" t="s">
+        <v>73</v>
+      </c>
+      <c r="I117">
+        <v>0.48</v>
+      </c>
+      <c r="J117">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K117">
+        <v>0.79</v>
+      </c>
+      <c r="L117">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>4</v>
+      </c>
+      <c r="C118" t="s">
+        <v>81</v>
+      </c>
+      <c r="D118">
+        <v>-609.27070000000003</v>
+      </c>
+      <c r="E118">
+        <v>500</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H118" t="s">
+        <v>73</v>
+      </c>
+      <c r="I118">
+        <v>0.48</v>
+      </c>
+      <c r="J118">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K118">
+        <v>0.79</v>
+      </c>
+      <c r="L118">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>4</v>
+      </c>
+      <c r="C119" t="s">
+        <v>27</v>
+      </c>
+      <c r="D119">
+        <v>-420.56108999999998</v>
+      </c>
+      <c r="E119">
+        <v>500</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H119" t="s">
+        <v>73</v>
+      </c>
+      <c r="I119">
+        <v>0.48</v>
+      </c>
+      <c r="J119">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="K119">
+        <v>0.79</v>
+      </c>
+      <c r="L119">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s">
+        <v>36</v>
+      </c>
+      <c r="D120">
+        <v>-486.26867700000003</v>
+      </c>
+      <c r="E120">
+        <v>500</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H120" t="s">
+        <v>73</v>
+      </c>
+      <c r="I120">
+        <v>0.48</v>
+      </c>
+      <c r="J120">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="K120">
+        <v>0.79</v>
+      </c>
+      <c r="L120">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s">
+        <v>87</v>
+      </c>
+      <c r="D121">
+        <v>-581.00440000000003</v>
+      </c>
+      <c r="E121">
+        <v>500</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H121" t="s">
+        <v>73</v>
+      </c>
+      <c r="I121">
+        <v>0.48</v>
+      </c>
+      <c r="J121">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="K121">
+        <v>0.79</v>
+      </c>
+      <c r="L121">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>4</v>
+      </c>
+      <c r="C122" t="s">
+        <v>26</v>
+      </c>
+      <c r="D122">
+        <v>-517.9452</v>
+      </c>
+      <c r="E122">
+        <v>500</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H122" t="s">
+        <v>73</v>
+      </c>
+      <c r="I122">
+        <v>0.48</v>
+      </c>
+      <c r="J122">
+        <v>0.77149999999999996</v>
+      </c>
+      <c r="K122">
+        <v>0.79</v>
+      </c>
+      <c r="L122">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>665.82399999999996</v>
+      </c>
+      <c r="B123">
+        <v>4</v>
+      </c>
+      <c r="C123" t="s">
+        <v>88</v>
+      </c>
+      <c r="D123">
+        <v>-617.20799999999997</v>
+      </c>
+      <c r="E123">
+        <v>500</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H123" t="s">
+        <v>73</v>
+      </c>
+      <c r="I123">
+        <v>0.48</v>
+      </c>
+      <c r="J123">
+        <v>0.77149999999999996</v>
+      </c>
+      <c r="K123">
+        <v>0.79</v>
+      </c>
+      <c r="L123">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="E125">
+        <v>500</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H125" t="s">
+        <v>12</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+      <c r="K125">
+        <v>1</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>500</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H126" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="E127">
+        <v>500</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H127" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>500</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H128" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="E129">
+        <v>500</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H129" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alte und überflüssige Dokumente entfernt
</commit_message>
<xml_diff>
--- a/PSO_Auswertung.xlsx
+++ b/PSO_Auswertung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="90">
   <si>
     <t>Testfunktion</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>23 von 100.000</t>
+  </si>
+  <si>
+    <t>0 bis 3</t>
   </si>
 </sst>
 </file>
@@ -301,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,12 +314,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -343,8 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -659,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H132" sqref="H132"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,12 +990,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>26</v>
-      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -3943,38 +3933,38 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="96" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="3">
+    <row r="96" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="6">
         <v>4</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="6">
         <v>-623.41399999999999</v>
       </c>
-      <c r="E96" s="3">
-        <v>500</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G96" s="5" t="s">
+      <c r="E96" s="6">
+        <v>500</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G96" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H96" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I96" s="3">
+      <c r="H96" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I96" s="6">
         <v>0.49</v>
       </c>
-      <c r="J96" s="3">
+      <c r="J96" s="6">
         <v>0.79</v>
       </c>
-      <c r="K96" s="3">
+      <c r="K96" s="6">
         <v>0.79</v>
       </c>
-      <c r="L96" s="3">
+      <c r="L96" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -4363,38 +4353,38 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="108" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="3">
+    <row r="108" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="6">
         <v>4</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="6">
         <v>-623.37649999999996</v>
       </c>
-      <c r="E108" s="3">
-        <v>500</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G108" s="5" t="s">
+      <c r="E108" s="6">
+        <v>500</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G108" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H108" s="3" t="s">
+      <c r="H108" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I108" s="3">
+      <c r="I108" s="6">
         <v>0.48</v>
       </c>
-      <c r="J108" s="3">
+      <c r="J108" s="6">
         <v>0.78</v>
       </c>
-      <c r="K108" s="3">
+      <c r="K108" s="6">
         <v>0.79</v>
       </c>
-      <c r="L108" s="3">
+      <c r="L108" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -4433,38 +4423,38 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="110" spans="2:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="9">
+    <row r="110" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="3">
         <v>4</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C110" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="3">
         <v>-637.54690000000005</v>
       </c>
-      <c r="E110" s="9">
-        <v>500</v>
-      </c>
-      <c r="F110" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G110" s="10" t="s">
+      <c r="E110" s="3">
+        <v>500</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G110" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H110" s="9" t="s">
+      <c r="H110" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I110" s="9">
+      <c r="I110" s="3">
         <v>0.48</v>
       </c>
-      <c r="J110" s="9">
+      <c r="J110" s="3">
         <v>0.77</v>
       </c>
-      <c r="K110" s="9">
+      <c r="K110" s="3">
         <v>0.79</v>
       </c>
-      <c r="L110" s="9">
+      <c r="L110" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -4643,38 +4633,38 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="3">
+    <row r="116" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="6">
         <v>4</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D116" s="6">
         <v>-623.41463999999996</v>
       </c>
-      <c r="E116" s="3">
-        <v>500</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G116" s="5" t="s">
+      <c r="E116" s="6">
+        <v>500</v>
+      </c>
+      <c r="F116" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G116" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H116" s="3" t="s">
+      <c r="H116" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I116" s="3">
+      <c r="I116" s="6">
         <v>0.48</v>
       </c>
-      <c r="J116" s="3">
+      <c r="J116" s="6">
         <v>0.77200000000000002</v>
       </c>
-      <c r="K116" s="3">
+      <c r="K116" s="6">
         <v>0.79</v>
       </c>
-      <c r="L116" s="3">
+      <c r="L116" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -4934,14 +4924,20 @@
       <c r="B125">
         <v>2</v>
       </c>
+      <c r="C125" t="s">
+        <v>20</v>
+      </c>
+      <c r="D125">
+        <v>28.080300000000001</v>
+      </c>
       <c r="E125">
         <v>500</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H125" t="s">
         <v>12</v>
@@ -4953,7 +4949,7 @@
         <v>1</v>
       </c>
       <c r="K125">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="L125">
         <v>0</v>
@@ -4963,68 +4959,770 @@
       <c r="B126">
         <v>2</v>
       </c>
+      <c r="C126" t="s">
+        <v>20</v>
+      </c>
+      <c r="D126">
+        <v>27.207000000000001</v>
+      </c>
       <c r="E126">
         <v>500</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H126" t="s">
         <v>12</v>
+      </c>
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+      <c r="K126">
+        <v>0.4</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>2</v>
       </c>
+      <c r="C127" t="s">
+        <v>20</v>
+      </c>
+      <c r="D127">
+        <v>26.951637900000001</v>
+      </c>
       <c r="E127">
         <v>500</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H127" t="s">
         <v>12</v>
+      </c>
+      <c r="I127">
+        <v>1</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+      <c r="K127">
+        <v>0.4</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>2</v>
       </c>
+      <c r="C128" t="s">
+        <v>20</v>
+      </c>
+      <c r="D128">
+        <v>26.961115100000001</v>
+      </c>
       <c r="E128">
         <v>500</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H128" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+      <c r="K128">
+        <v>0.4</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>2</v>
       </c>
+      <c r="C129" t="s">
+        <v>67</v>
+      </c>
+      <c r="D129">
+        <v>27.726647700000001</v>
+      </c>
       <c r="E129">
         <v>500</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H129" t="s">
         <v>12</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <v>1</v>
+      </c>
+      <c r="K129">
+        <v>0.4</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
+        <v>27</v>
+      </c>
+      <c r="D130">
+        <v>27.505325200000001</v>
+      </c>
+      <c r="E130">
+        <v>500</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H130" t="s">
+        <v>12</v>
+      </c>
+      <c r="I130">
+        <v>1</v>
+      </c>
+      <c r="J130">
+        <v>1</v>
+      </c>
+      <c r="K130">
+        <v>0.45</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
+        <v>20</v>
+      </c>
+      <c r="D131">
+        <v>27.716579299999999</v>
+      </c>
+      <c r="E131">
+        <v>500</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H131" t="s">
+        <v>12</v>
+      </c>
+      <c r="I131">
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <v>1</v>
+      </c>
+      <c r="K131">
+        <v>0.45</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
+        <v>20</v>
+      </c>
+      <c r="D132">
+        <v>28.532518490000001</v>
+      </c>
+      <c r="E132">
+        <v>500</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H132" t="s">
+        <v>12</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+      <c r="K132">
+        <v>0.41</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>26</v>
+      </c>
+      <c r="D133">
+        <v>27.066679000000001</v>
+      </c>
+      <c r="E133">
+        <v>500</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H133" t="s">
+        <v>12</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+      <c r="K133">
+        <v>0.41</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>27</v>
+      </c>
+      <c r="D134">
+        <v>36.369959999999999</v>
+      </c>
+      <c r="E134">
+        <v>500</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H134" t="s">
+        <v>12</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+      <c r="K134">
+        <v>0.39</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="C135" t="s">
+        <v>34</v>
+      </c>
+      <c r="D135">
+        <v>28.84181354</v>
+      </c>
+      <c r="E135">
+        <v>500</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H135" t="s">
+        <v>12</v>
+      </c>
+      <c r="I135">
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <v>1</v>
+      </c>
+      <c r="K135">
+        <v>0.39</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="3">
+        <v>2</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" s="3">
+        <v>26.815667000000001</v>
+      </c>
+      <c r="E136" s="3">
+        <v>500</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I136" s="3">
+        <v>1</v>
+      </c>
+      <c r="J136" s="3">
+        <v>1</v>
+      </c>
+      <c r="K136" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="L136" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>2</v>
+      </c>
+      <c r="C137" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137">
+        <v>26.904748699999999</v>
+      </c>
+      <c r="E137">
+        <v>500</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H137" t="s">
+        <v>12</v>
+      </c>
+      <c r="I137">
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137">
+        <v>0.39</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>2</v>
+      </c>
+      <c r="C138" t="s">
+        <v>20</v>
+      </c>
+      <c r="D138">
+        <v>27.669346999999998</v>
+      </c>
+      <c r="E138">
+        <v>500</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H138" t="s">
+        <v>12</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+      <c r="K138">
+        <v>0.39</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139">
+        <v>27.333030000000001</v>
+      </c>
+      <c r="E139">
+        <v>500</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H139" t="s">
+        <v>12</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+      <c r="K139">
+        <v>0.38</v>
+      </c>
+      <c r="L139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>2</v>
+      </c>
+      <c r="C140" t="s">
+        <v>28</v>
+      </c>
+      <c r="D140">
+        <v>27.232130399999999</v>
+      </c>
+      <c r="E140">
+        <v>500</v>
+      </c>
+      <c r="F140" t="s">
+        <v>89</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H140" t="s">
+        <v>12</v>
+      </c>
+      <c r="I140">
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <v>1</v>
+      </c>
+      <c r="K140">
+        <v>0.38</v>
+      </c>
+      <c r="L140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>2</v>
+      </c>
+      <c r="C141" t="s">
+        <v>31</v>
+      </c>
+      <c r="D141">
+        <v>29.478127700000002</v>
+      </c>
+      <c r="E141">
+        <v>500</v>
+      </c>
+      <c r="F141" t="s">
+        <v>89</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H141" t="s">
+        <v>12</v>
+      </c>
+      <c r="I141">
+        <v>1</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+      <c r="K141">
+        <v>0.38</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>2</v>
+      </c>
+      <c r="C142" t="s">
+        <v>20</v>
+      </c>
+      <c r="D142">
+        <v>27.975473399999998</v>
+      </c>
+      <c r="E142">
+        <v>500</v>
+      </c>
+      <c r="F142" t="s">
+        <v>89</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H142" t="s">
+        <v>12</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+      <c r="K142">
+        <v>0.38</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>2</v>
+      </c>
+      <c r="C143" t="s">
+        <v>27</v>
+      </c>
+      <c r="D143">
+        <v>27.931905400000002</v>
+      </c>
+      <c r="E143">
+        <v>500</v>
+      </c>
+      <c r="F143" t="s">
+        <v>89</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H143" t="s">
+        <v>12</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>2</v>
+      </c>
+      <c r="C144" t="s">
+        <v>27</v>
+      </c>
+      <c r="D144">
+        <v>26.919924000000002</v>
+      </c>
+      <c r="E144">
+        <v>500</v>
+      </c>
+      <c r="F144" t="s">
+        <v>89</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H144" t="s">
+        <v>12</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+      <c r="K144">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>2</v>
+      </c>
+      <c r="C145" t="s">
+        <v>27</v>
+      </c>
+      <c r="D145">
+        <v>27.0022564</v>
+      </c>
+      <c r="E145">
+        <v>500</v>
+      </c>
+      <c r="F145" t="s">
+        <v>89</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H145" t="s">
+        <v>12</v>
+      </c>
+      <c r="I145">
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+      <c r="K145">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>2</v>
+      </c>
+      <c r="C146" t="s">
+        <v>27</v>
+      </c>
+      <c r="D146">
+        <v>26.885134129000001</v>
+      </c>
+      <c r="E146">
+        <v>500</v>
+      </c>
+      <c r="F146" t="s">
+        <v>89</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H146" t="s">
+        <v>12</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+      <c r="K146">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="L146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>2</v>
+      </c>
+      <c r="C147" t="s">
+        <v>20</v>
+      </c>
+      <c r="D147">
+        <v>27.80823775</v>
+      </c>
+      <c r="E147">
+        <v>500</v>
+      </c>
+      <c r="F147" t="s">
+        <v>89</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H147" t="s">
+        <v>12</v>
+      </c>
+      <c r="I147">
+        <v>1</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+      <c r="K147">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="L147">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>